<commit_message>
feat: Add initial Streamlit UI components, image assets, configuration files, and supporting scripts for the triage evaluation study application.
</commit_message>
<xml_diff>
--- a/config/study_content_pack.xlsx
+++ b/config/study_content_pack.xlsx
@@ -623,7 +623,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Red</t>
+          <t>Orange</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Yellow</t>
+          <t>Green</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Blue</t>
         </is>
       </c>
     </row>
@@ -674,7 +674,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>White</t>
         </is>
       </c>
     </row>
@@ -842,7 +842,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -858,183 +858,2791 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Patient_Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Scenario</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Is_Tutorial</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Avatar_File</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Visible_Text</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>walk_Text</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>voice_Text</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>pulse_Text</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>rr_Text</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>airway_Text</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Gold_Standard_Raw</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Gold_Standard_Normalized</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Hidden_ISS</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Critical_Failure_Type</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>tourniquet_Text</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Gold_Standard_Normalized</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Avatar_File</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>tut_01</t>
+          <t>ent_01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Tutorial</t>
-        </is>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Male, 30s. Sitting on curb. Holding arm.</t>
-        </is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>ent_01.png</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Male, 40s. Sitting on a chair, covered in dust, minor bleeding from forehead. Anxious.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>Yes, I can walk.</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>I'm okay, just scared.'</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 95bpm.</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>18/min</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>P3 (Walking)</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
           <t>Green</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>default.png</t>
-        </is>
-      </c>
+      <c r="N2" t="n">
+        <v>5</v>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ent_01</t>
+          <t>ent_02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Chloe</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Entrapment</t>
         </is>
       </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Female, 40s. Legs pinned under rubble. Screaming.</t>
-        </is>
+      <c r="D3" t="b">
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>I can't move!</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+          <t>ent_02.png</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Female, 30s. Lower body pinned by a concrete slab. Conscious, screaming in pain.</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>I can't move my legs.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>It's crushing me! Get it off!'</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>Radial pulse present, 110bpm.</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>24/min</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Cat 3 (Urgent)</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
           <t>Yellow</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>default.png</t>
-        </is>
-      </c>
+      <c r="N3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>vio_01</t>
+          <t>ent_03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Violence</t>
-        </is>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Male, GSW to chest. Unconscious. Silent.</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+          <t>Marcus</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ent_03.png</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Male, 60s. Unresponsive, trapped chest under a beam. Shallow, labored breathing.</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Obstructed. Blood in airway.</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr"/>
+          <t>Weak radial pulse, 135bpm.</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Agonal, 6/min</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
+          <t>Snoring</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Priority 1 (Red)</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
           <t>Red</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>default.png</t>
-        </is>
-      </c>
+      <c r="N4" t="n">
+        <v>55</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Preventable Death</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ent_04</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Elena</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ent_04.png</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Female, 50s. Completely buried under debris. Silent and still.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Dead</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>75</v>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ent_05</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ent_05.png</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Male, 20s. Pinned arm with severe, spurting bleeding. Awake, pale, and rapidly deteriorating.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>I can't move.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>I'm going to pass out.'</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Thready radial pulse, 150bpm.</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Rapid, 40/min</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Cat 1 (Immediate)</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>60</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Preventable Death</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ent_06</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ben</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ent_06.png</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Male, 50s. Complaining of chest pain and difficulty breathing after a wall collapse.</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>I can't walk, too painful.</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>My chest hurts to breathe.'</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 120bpm.</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Labored, 35/min</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Cat 2 (Imminent)</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="N7" t="n">
+        <v>30</v>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ent_07</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Kate</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ent_07.png</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Female, 40s. Trapped but alert, with a simple fracture to her arm. Moderate pain.</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>I can't move.</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>My arm is broken.'</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 90bpm.</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>18/min</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Cat 3 (Urgent)</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>12</v>
+      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ent_08</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>ent_08.png</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Male, 20s. Pinched leg, complaining of intense numbness and swelling.</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>I can't move my leg.</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>It's huge, I can't feel it.'</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 100bpm.</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>20/min</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Cat 3 (Urgent)</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>25</v>
+      </c>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ent_09</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Sophie</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>ent_09.png</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Female, 70s. Sitting on a pile of rubble. Crying, no visible major injuries.</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Yes, I can walk.</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Where is my husband?'</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 105bpm.</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>22/min</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Cat 4 (Semi-Urgent)</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>4</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Over-triage</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ent_10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Liam</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>ent_10.png</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Male, 30s. Half-buried in dust/dirt, alert but disoriented.</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>I can't move.</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Help me get out.'</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 115bpm.</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>28/min</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Cat 2 (Imminent)</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>45</v>
+      </c>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ent_11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Mia</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>ent_11.png</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Female, 20s. Found underneath a collapsed ceiling, silent, no pulse, pupils fixed and dilated.</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Dead</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>75</v>
+      </c>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ent_12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>ent_12.png</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Male, 50s. Trapped under a car. Conscious, pale. Complaining of severe pain and pelvic pressure.</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>I can't move.</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>I feel lightheaded.'</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Thready radial pulse, 130bpm.</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Rapid, 35/min</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Priority 1 (Red)</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>40</v>
+      </c>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ent_13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Ruby</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>ent_13.png</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Female, 30s. Walking wounded, minor lacerations, a bit shaky.</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Yes, I can walk.</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Is the shaking over?'</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 88bpm.</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>16/min</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Cat 5 (Non-Urgent)</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>2</v>
+      </c>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ent_14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Sam</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>ent_14.png</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Male, 40s. Trapped by legs. Calmly asking for water.</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>I can't move.</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Can I have some water?'</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 90bpm.</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>18/min</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Cat 3 (Urgent)</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>10</v>
+      </c>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ent_15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Tom</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>ent_15.png</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Male, 20s. Unconscious, pinned by a small bookcase. Gurgling sounds with each breath.</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Weak radial pulse, 125bpm.</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>30/min</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Obstructed. Gurgling.</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Priority 1 (Red)</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
+        <v>35</v>
+      </c>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ent_16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Zoe</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>ent_16.png</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Female, 60s. Pinched arm, severe dust inhalation causing coughing. Alert and anxious.</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>I can't move.</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>I'm coughing up dust.'</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 100bpm.</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Labored, 28/min</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Cat 3 (Urgent)</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>16</v>
+      </c>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ent_17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>William</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>ent_17.png</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Male, 30s. Unresponsive, GSW to the back of the head (pre-existing, old wound). Cold to touch.</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Dead</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
+        <v>75</v>
+      </c>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ent_18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Ava</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>ent_18.png</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Female, 20s. Trapped hand under metal, minor bleeding. Alert and able to talk.</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>I can't move my hand.</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>I need my hand out.'</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 98bpm.</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>20/min</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Cat 3 (Urgent)</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>18</v>
+      </c>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ent_19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Harry</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>ent_19.png</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Male, 40s. Pinched under roof wreckage. Confused, not responding to commands.</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>I can't move.</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Thready radial pulse, 140bpm.</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Rapid, shallow (38/min)</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Cat 1 (Immediate)</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
+        <v>58</v>
+      </c>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ent_20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Isabel</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Entrapment</t>
+        </is>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>ent_20.png</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Female, 50s. Visible crush injury to the face, unconscious. No respiratory effort.</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Dead</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="N21" t="n">
+        <v>75</v>
+      </c>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>vio_01</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>vio_01.png</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Male, 30s. Lying supine. GSW to the upper chest, small amount of bubbling at the wound site.</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Weak radial pulse, 130bpm.</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Rapid, 40/min</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Priority 1 (Red)</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="N22" t="n">
+        <v>50</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Preventable Death</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>vio_02</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Beth</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>vio_02.png</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Female, 20s. GSW to the thigh, moderate venous bleeding. Alert, holding the wound.</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>I can walk, but it hurts.</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>I'm hit! I need pressure.'</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 115bpm.</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>28/min</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Cat 3 (Urgent)</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="N23" t="n">
+        <v>20</v>
+      </c>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>vio_03</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Charles</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>vio_03.png</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Male, 40s. Unresponsive, multiple GSWs to the torso and head. No signs of life.</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Dead</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="N24" t="n">
+        <v>75</v>
+      </c>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>vio_04</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Denise</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>vio_04.png</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Female, 50s. Shrapnel wounds to the lower leg. Able to walk, limping significantly.</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Yes, I can walk.</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>I can't put weight on it.'</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 95bpm.</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>20/min</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>P3 (Walking)</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="N25" t="n">
+        <v>10</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Over-triage</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>vio_05</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Ethan</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>vio_05.png</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Male, 20s. GSW to the neck, massive blood loss. Unconscious and pale.</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Absent radial pulse, Carotid 150bpm.</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Rapid, shallow (45/min)</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Obstructed. Snoring.</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Cat 1 (Immediate)</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="N26" t="n">
+        <v>65</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Preventable Death</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>vio_06</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Fiona</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>vio_06.png</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Female, 30s. Crying, hiding under a desk. No visible physical injuries.</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Yes, I can walk.</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>They're still out there!'</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 110bpm.</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>25/min</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Cat 5 (Non-Urgent)</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Over-triage</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>vio_07</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Gary</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>vio_07.png</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Male, 60s. Shrapnel wounds to the back and head. Conscious, oriented, but complaining of headache.</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>I can walk, but I'm dizzy.</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>I feel sick to my stomach.'</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 100bpm.</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>22/min</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Cat 3 (Urgent)</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="N28" t="n">
+        <v>15</v>
+      </c>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>vio_08</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Helen</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>vio_08.png</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Female, 40s. Lying on the floor, GSW to the abdomen. Silent but moaning when moved.</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>I can't move.</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Thready radial pulse, 140bpm.</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Rapid, 40/min</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Priority 1 (Red)</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="N29" t="n">
+        <v>60</v>
+      </c>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>vio_09</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Isaac</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>vio_09.png</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Male, 50s. GSW to the arm, not bleeding heavily. Alert, pale, and worried.</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Yes, I can walk.</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Just my arm is hit.'</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 105bpm.</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>20/min</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Cat 3 (Urgent)</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="N30" t="n">
+        <v>12</v>
+      </c>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>vio_10</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Jasmine</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>vio_10.png</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Female, 20s. Unresponsive. GSW to the pelvis, moderate bleeding.</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Weak radial pulse, 135bpm.</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Shallow, 35/min</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Cat 2 (Imminent)</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="N31" t="n">
+        <v>52</v>
+      </c>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>vio_11</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Karl</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D32" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>vio_11.png</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Male, 30s. Walking around, helping people. No visible injuries.</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Yes, I can walk.</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>I'm a first-aider.'</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 80bpm.</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>14/min</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>P3 (Walking)</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>vio_12</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Lana</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>vio_12.png</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Female, 40s. Multiple shrapnel wounds to the back and legs. Conscious, in severe pain.</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>I can't move.</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>The pain is too much.'</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 120bpm.</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>30/min</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Cat 2 (Imminent)</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="N33" t="n">
+        <v>42</v>
+      </c>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>vio_13</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>vio_13.png</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Male, 60s. Unresponsive. Massive bleeding from a large shrapnel wound to the head.</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Dead</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="N34" t="n">
+        <v>75</v>
+      </c>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>vio_14</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Nina</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>vio_14.png</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Female, 30s. Lying on the ground. Unconscious, not responding to painful stimuli.</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Thready radial pulse, 140bpm.</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Rapid, 40/min</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Obstructed. Gurgling.</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Priority 1 (Red)</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="N35" t="n">
+        <v>55</v>
+      </c>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>vio_15</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Oscar</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>vio_15.png</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Male, 20s. GSW to the arm. Alert, moderate bleeding, sitting against a wall.</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>I can walk, if I had to.</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>It stings, but I'll be fine.'</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 100bpm.</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>20/min</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Cat 3 (Urgent)</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="N36" t="n">
+        <v>14</v>
+      </c>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>vio_16</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Paula</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D37" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>vio_16.png</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Female, 50s. GSW to the knee. Alert, unable to walk, stable vitals.</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>I can't stand up.</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>I think my leg is shattered.'</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 92bpm.</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>18/min</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Cat 3 (Urgent)</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="N37" t="n">
+        <v>18</v>
+      </c>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>vio_17</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Roger</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>vio_17.png</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Male, 40s. Lying on side. Unresponsive. GSW to the abdomen.</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Weak radial pulse, 130bpm.</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Shallow, 35/min</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Cat 2 (Imminent)</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="N38" t="n">
+        <v>48</v>
+      </c>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>vio_18</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Shelly</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>vio_18.png</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Female, 30s. GSW to the face. Awake, unable to speak clearly due to injury.</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Yes, I can walk.</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>...' (Mumbling)</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 110bpm.</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>25/min</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Cat 4 (Semi-Urgent)</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="N39" t="n">
+        <v>8</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>Over-triage</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>vio_19</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Terry</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D40" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>vio_19.png</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Male, 20s. GSW to the shoulder, minimal bleeding. Anxious.</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Yes, I can walk.</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Just my arm.'</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Radial pulse present, 105bpm.</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>22/min</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Clear</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>Cat 3 (Urgent)</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="N40" t="n">
+        <v>10</v>
+      </c>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>vio_20</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Ursula</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Violence</t>
+        </is>
+      </c>
+      <c r="D41" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>vio_20.png</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Female, 60s. Unresponsive. GSW to the head. Cold to the touch.</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Dead</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="N41" t="n">
+        <v>75</v>
+      </c>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: Add script to fix invalid Normalized_Value entries in study_content_pack.xlsx
</commit_message>
<xml_diff>
--- a/config/study_content_pack.xlsx
+++ b/config/study_content_pack.xlsx
@@ -623,7 +623,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Orange</t>
+          <t>Yellow</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Blue</t>
+          <t>Yellow</t>
         </is>
       </c>
     </row>
@@ -674,7 +674,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Green</t>
         </is>
       </c>
     </row>
@@ -999,8 +999,6 @@
       <c r="N2" t="n">
         <v>5</v>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1069,8 +1067,6 @@
       <c r="N3" t="n">
         <v>20</v>
       </c>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1101,8 +1097,6 @@
           <t>Male, 60s. Unresponsive, trapped chest under a beam. Shallow, labored breathing.</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
           <t>Weak radial pulse, 135bpm.</t>
@@ -1136,7 +1130,6 @@
           <t>Preventable Death</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1167,8 +1160,6 @@
           <t>Female, 50s. Completely buried under debris. Silent and still.</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>Absent</t>
@@ -1197,8 +1188,6 @@
       <c r="N5" t="n">
         <v>75</v>
       </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1272,7 +1261,6 @@
           <t>Preventable Death</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1341,8 +1329,6 @@
       <c r="N7" t="n">
         <v>30</v>
       </c>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1411,8 +1397,6 @@
       <c r="N8" t="n">
         <v>12</v>
       </c>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1481,8 +1465,6 @@
       <c r="N9" t="n">
         <v>25</v>
       </c>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1556,7 +1538,6 @@
           <t>Over-triage</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1625,8 +1606,6 @@
       <c r="N11" t="n">
         <v>45</v>
       </c>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1657,8 +1636,6 @@
           <t>Female, 20s. Found underneath a collapsed ceiling, silent, no pulse, pupils fixed and dilated.</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
           <t>Absent</t>
@@ -1687,8 +1664,6 @@
       <c r="N12" t="n">
         <v>75</v>
       </c>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1757,8 +1732,6 @@
       <c r="N13" t="n">
         <v>40</v>
       </c>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1827,8 +1800,6 @@
       <c r="N14" t="n">
         <v>2</v>
       </c>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1897,8 +1868,6 @@
       <c r="N15" t="n">
         <v>10</v>
       </c>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1929,8 +1898,6 @@
           <t>Male, 20s. Unconscious, pinned by a small bookcase. Gurgling sounds with each breath.</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
           <t>Weak radial pulse, 125bpm.</t>
@@ -1959,8 +1926,6 @@
       <c r="N16" t="n">
         <v>35</v>
       </c>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2029,8 +1994,6 @@
       <c r="N17" t="n">
         <v>16</v>
       </c>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2061,8 +2024,6 @@
           <t>Male, 30s. Unresponsive, GSW to the back of the head (pre-existing, old wound). Cold to touch.</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
           <t>Absent</t>
@@ -2091,8 +2052,6 @@
       <c r="N18" t="n">
         <v>75</v>
       </c>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2161,8 +2120,6 @@
       <c r="N19" t="n">
         <v>18</v>
       </c>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2198,7 +2155,6 @@
           <t>I can't move.</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
           <t>Thready radial pulse, 140bpm.</t>
@@ -2227,8 +2183,6 @@
       <c r="N20" t="n">
         <v>58</v>
       </c>
-      <c r="O20" t="inlineStr"/>
-      <c r="P20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2259,8 +2213,6 @@
           <t>Female, 50s. Visible crush injury to the face, unconscious. No respiratory effort.</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
           <t>Absent</t>
@@ -2289,8 +2241,6 @@
       <c r="N21" t="n">
         <v>75</v>
       </c>
-      <c r="O21" t="inlineStr"/>
-      <c r="P21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2321,8 +2271,6 @@
           <t>Male, 30s. Lying supine. GSW to the upper chest, small amount of bubbling at the wound site.</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr">
         <is>
           <t>Weak radial pulse, 130bpm.</t>
@@ -2356,7 +2304,6 @@
           <t>Preventable Death</t>
         </is>
       </c>
-      <c r="P22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2425,8 +2372,6 @@
       <c r="N23" t="n">
         <v>20</v>
       </c>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2457,8 +2402,6 @@
           <t>Male, 40s. Unresponsive, multiple GSWs to the torso and head. No signs of life.</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr">
         <is>
           <t>Absent</t>
@@ -2487,8 +2430,6 @@
       <c r="N24" t="n">
         <v>75</v>
       </c>
-      <c r="O24" t="inlineStr"/>
-      <c r="P24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2562,7 +2503,6 @@
           <t>Over-triage</t>
         </is>
       </c>
-      <c r="P25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2593,8 +2533,6 @@
           <t>Male, 20s. GSW to the neck, massive blood loss. Unconscious and pale.</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr">
         <is>
           <t>Absent radial pulse, Carotid 150bpm.</t>
@@ -2628,7 +2566,6 @@
           <t>Preventable Death</t>
         </is>
       </c>
-      <c r="P26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2702,7 +2639,6 @@
           <t>Over-triage</t>
         </is>
       </c>
-      <c r="P27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2771,8 +2707,6 @@
       <c r="N28" t="n">
         <v>15</v>
       </c>
-      <c r="O28" t="inlineStr"/>
-      <c r="P28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2808,7 +2742,6 @@
           <t>I can't move.</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
           <t>Thready radial pulse, 140bpm.</t>
@@ -2837,8 +2770,6 @@
       <c r="N29" t="n">
         <v>60</v>
       </c>
-      <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2907,8 +2838,6 @@
       <c r="N30" t="n">
         <v>12</v>
       </c>
-      <c r="O30" t="inlineStr"/>
-      <c r="P30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2939,8 +2868,6 @@
           <t>Female, 20s. Unresponsive. GSW to the pelvis, moderate bleeding.</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr">
         <is>
           <t>Weak radial pulse, 135bpm.</t>
@@ -2969,8 +2896,6 @@
       <c r="N31" t="n">
         <v>52</v>
       </c>
-      <c r="O31" t="inlineStr"/>
-      <c r="P31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3039,8 +2964,6 @@
       <c r="N32" t="n">
         <v>0</v>
       </c>
-      <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3109,8 +3032,6 @@
       <c r="N33" t="n">
         <v>42</v>
       </c>
-      <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3141,8 +3062,6 @@
           <t>Male, 60s. Unresponsive. Massive bleeding from a large shrapnel wound to the head.</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr">
         <is>
           <t>Absent</t>
@@ -3171,8 +3090,6 @@
       <c r="N34" t="n">
         <v>75</v>
       </c>
-      <c r="O34" t="inlineStr"/>
-      <c r="P34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3203,8 +3120,6 @@
           <t>Female, 30s. Lying on the ground. Unconscious, not responding to painful stimuli.</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr">
         <is>
           <t>Thready radial pulse, 140bpm.</t>
@@ -3233,8 +3148,6 @@
       <c r="N35" t="n">
         <v>55</v>
       </c>
-      <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3303,8 +3216,6 @@
       <c r="N36" t="n">
         <v>14</v>
       </c>
-      <c r="O36" t="inlineStr"/>
-      <c r="P36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3373,8 +3284,6 @@
       <c r="N37" t="n">
         <v>18</v>
       </c>
-      <c r="O37" t="inlineStr"/>
-      <c r="P37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3405,8 +3314,6 @@
           <t>Male, 40s. Lying on side. Unresponsive. GSW to the abdomen.</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr">
         <is>
           <t>Weak radial pulse, 130bpm.</t>
@@ -3435,8 +3342,6 @@
       <c r="N38" t="n">
         <v>48</v>
       </c>
-      <c r="O38" t="inlineStr"/>
-      <c r="P38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3510,7 +3415,6 @@
           <t>Over-triage</t>
         </is>
       </c>
-      <c r="P39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3579,8 +3483,6 @@
       <c r="N40" t="n">
         <v>10</v>
       </c>
-      <c r="O40" t="inlineStr"/>
-      <c r="P40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3611,8 +3513,6 @@
           <t>Female, 60s. Unresponsive. GSW to the head. Cold to the touch.</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr">
         <is>
           <t>Absent</t>
@@ -3641,8 +3541,6 @@
       <c r="N41" t="n">
         <v>75</v>
       </c>
-      <c r="O41" t="inlineStr"/>
-      <c r="P41" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>